<commit_message>
converted to xlsx take-2
</commit_message>
<xml_diff>
--- a/HIR-MEZUNIYET.xlsx
+++ b/HIR-MEZUNIYET.xlsx
@@ -1,25 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
-  <workbookPr dateCompatibility="0" defaultThemeVersion="124226"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/naimcinar/Projects/hir-mezuniyet-kontrol/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C64305B-6315-E44E-8389-4FB752117F5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{90FC7786-813C-E045-B133-65963984E22F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="760" windowWidth="25060" windowHeight="16480" xr2:uid="{12270DE2-0529-8240-A4E8-A2B8FED8975C}"/>
+    <workbookView xWindow="120" yWindow="760" windowWidth="25060" windowHeight="16480" xr2:uid="{C801968A-2E07-2744-97E1-6F35C38B86E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -36,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="180" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="82">
   <si>
     <t>I. YARIYIL</t>
   </si>
@@ -287,7 +284,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="188" formatCode="0.0"/>
     <numFmt numFmtId="190" formatCode="#,##0.0"/>
@@ -434,15 +431,15 @@
   </fills>
   <borders count="3">
     <border>
-      <start/>
-      <end/>
+      <left/>
+      <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <start/>
-      <end/>
+      <left/>
+      <right/>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -450,8 +447,8 @@
       <diagonal/>
     </border>
     <border>
-      <start/>
-      <end/>
+      <left/>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -686,7 +683,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
     <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
@@ -805,22 +802,22 @@
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0%">
+            <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="50%"/>
-                <a:satMod val="300%"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="35%">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:tint val="37%"/>
-                <a:satMod val="300%"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100%">
+            <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15%"/>
-                <a:satMod val="350%"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -828,22 +825,22 @@
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0%">
+            <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51%"/>
-                <a:satMod val="130%"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="80%">
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:shade val="93%"/>
-                <a:satMod val="130%"/>
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100%">
+            <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94%"/>
-                <a:satMod val="135%"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -854,8 +851,8 @@
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
-              <a:shade val="95%"/>
-              <a:satMod val="105%"/>
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
             </a:schemeClr>
           </a:solidFill>
           <a:prstDash val="solid"/>
@@ -878,7 +875,7 @@
           <a:effectLst>
             <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="38%"/>
+                <a:alpha val="38000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -887,7 +884,7 @@
           <a:effectLst>
             <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="35%"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -896,7 +893,7 @@
           <a:effectLst>
             <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="35%"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -919,47 +916,47 @@
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0%">
+            <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="40%"/>
-                <a:satMod val="350%"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="40%">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="45%"/>
-                <a:shade val="99%"/>
-                <a:satMod val="350%"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100%">
+            <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20%"/>
-                <a:satMod val="255%"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50%" t="-80%" r="50%" b="180%"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0%">
+            <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="80%"/>
-                <a:satMod val="300%"/>
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100%">
+            <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="30%"/>
-                <a:satMod val="200%"/>
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50%" t="50%" r="50%" b="50%"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -971,7 +968,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2F2233D-C7C5-3840-A008-EAE7D55C506A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E95240E1-A168-5346-9E78-79A8407802B1}">
   <dimension ref="A1:O115"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A54" zoomScale="150" workbookViewId="0">

</xml_diff>